<commit_message>
data with feed columns
</commit_message>
<xml_diff>
--- a/data/d1/Amber.xlsx
+++ b/data/d1/Amber.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="34">
   <si>
     <t xml:space="preserve">Weeks</t>
   </si>
@@ -112,7 +112,10 @@
     <t xml:space="preserve">Egg Weight</t>
   </si>
   <si>
-    <t xml:space="preserve">Feed</t>
+    <t xml:space="preserve">Feed Offered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feed Refusal</t>
   </si>
   <si>
     <t xml:space="preserve">F</t>
@@ -221,7 +224,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -242,15 +245,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -343,10 +338,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BY19"/>
+  <dimension ref="A1:CU19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -361,38 +356,39 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="19" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="23" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="27" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="21" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="26" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="1" width="7.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="31" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="35" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="39" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="43" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="47" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="34" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="36" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="39" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="41" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="44" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="46" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="49" style="1" width="7.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="51" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="55" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="59" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="63" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="67" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="54" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="56" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="59" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="61" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="64" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="66" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="69" style="1" width="7.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="71" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="75" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="74" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="76" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="79" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="81" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="84" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="88" min="86" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="90" min="89" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="91" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="1" width="7.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -413,102 +409,119 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
       <c r="U1" s="3"/>
-      <c r="V1" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="Y1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
       <c r="AC1" s="3"/>
       <c r="AD1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
-      <c r="AH1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
-      <c r="AL1" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="AL1" s="3"/>
       <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
+      <c r="AN1" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="AO1" s="3"/>
-      <c r="AP1" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="AP1" s="3"/>
       <c r="AQ1" s="3"/>
       <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="AS1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
       <c r="AW1" s="3"/>
       <c r="AX1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AY1" s="3"/>
       <c r="AZ1" s="3"/>
       <c r="BA1" s="3"/>
-      <c r="BB1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="BC1" s="3"/>
+      <c r="BB1" s="3"/>
+      <c r="BC1" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="BD1" s="3"/>
       <c r="BE1" s="3"/>
-      <c r="BF1" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="BF1" s="3"/>
       <c r="BG1" s="3"/>
-      <c r="BH1" s="3"/>
+      <c r="BH1" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="BI1" s="3"/>
-      <c r="BJ1" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="BJ1" s="3"/>
       <c r="BK1" s="3"/>
       <c r="BL1" s="3"/>
-      <c r="BM1" s="3"/>
-      <c r="BN1" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="BM1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="BN1" s="3"/>
       <c r="BO1" s="3"/>
       <c r="BP1" s="3"/>
       <c r="BQ1" s="3"/>
       <c r="BR1" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="BS1" s="3"/>
       <c r="BT1" s="3"/>
       <c r="BU1" s="3"/>
-      <c r="BV1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="BW1" s="3"/>
+      <c r="BV1" s="3"/>
+      <c r="BW1" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="BX1" s="3"/>
       <c r="BY1" s="3"/>
+      <c r="BZ1" s="3"/>
+      <c r="CA1" s="3"/>
+      <c r="CB1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="CC1" s="3"/>
+      <c r="CD1" s="3"/>
+      <c r="CE1" s="3"/>
+      <c r="CF1" s="3"/>
+      <c r="CG1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="CH1" s="3"/>
+      <c r="CI1" s="3"/>
+      <c r="CJ1" s="3"/>
+      <c r="CK1" s="3"/>
+      <c r="CL1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="CM1" s="3"/>
+      <c r="CN1" s="3"/>
+      <c r="CO1" s="3"/>
+      <c r="CP1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -551,52 +564,52 @@
         <v>30</v>
       </c>
       <c r="N2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="X2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Z2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="AC2" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AD2" s="4" t="s">
         <v>27</v>
@@ -611,52 +624,52 @@
         <v>30</v>
       </c>
       <c r="AH2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AU2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AT2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AU2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AV2" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="AW2" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AX2" s="4" t="s">
         <v>27</v>
@@ -671,52 +684,52 @@
         <v>30</v>
       </c>
       <c r="BB2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="BC2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BD2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BE2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="BE2" s="4" t="s">
+      <c r="BF2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="BF2" s="4" t="s">
+      <c r="BG2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="BH2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="BG2" s="4" t="s">
+      <c r="BI2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="BH2" s="4" t="s">
+      <c r="BJ2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="BI2" s="4" t="s">
+      <c r="BK2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="BJ2" s="4" t="s">
+      <c r="BL2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="BM2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="BK2" s="4" t="s">
+      <c r="BN2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="BL2" s="4" t="s">
+      <c r="BO2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="BM2" s="4" t="s">
+      <c r="BP2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="BN2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="BO2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="BP2" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="BQ2" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="BR2" s="4" t="s">
         <v>27</v>
@@ -731,16 +744,67 @@
         <v>30</v>
       </c>
       <c r="BV2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="BW2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="BW2" s="4" t="s">
+      <c r="BX2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="BX2" s="4" t="s">
+      <c r="BY2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="BY2" s="4" t="s">
+      <c r="BZ2" s="4" t="s">
         <v>30</v>
+      </c>
+      <c r="CA2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="CB2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="CC2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="CD2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="CE2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="CF2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="CG2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="CH2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="CI2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="CJ2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="CK2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="CL2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="CM2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="CN2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="CO2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="CP2" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,417 +812,247 @@
         <v>1520</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5" t="n">
         <v>44784</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
       <c r="J3" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="0" t="n">
+      <c r="O3" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="0" t="n">
+      <c r="T3" s="0" t="n">
         <v>134</v>
       </c>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="0" t="n">
+      <c r="Y3" s="0" t="n">
         <v>237.3</v>
       </c>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="0" t="n">
+      <c r="AD3" s="0" t="n">
         <v>331</v>
       </c>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
-      <c r="AD3" s="0" t="n">
+      <c r="AI3" s="0" t="n">
         <v>440.1</v>
       </c>
-      <c r="AE3" s="7"/>
-      <c r="AF3" s="7"/>
-      <c r="AG3" s="7"/>
-      <c r="AH3" s="0" t="n">
+      <c r="AN3" s="0" t="n">
         <v>549.5</v>
       </c>
-      <c r="AI3" s="7"/>
-      <c r="AJ3" s="7"/>
-      <c r="AK3" s="7"/>
-      <c r="AL3" s="0" t="n">
+      <c r="AS3" s="0" t="n">
         <v>604.8</v>
       </c>
-      <c r="AM3" s="7"/>
-      <c r="AN3" s="7"/>
-      <c r="AO3" s="7"/>
-      <c r="AP3" s="0" t="n">
+      <c r="AX3" s="0" t="n">
         <v>609.2</v>
       </c>
-      <c r="AQ3" s="7"/>
-      <c r="AR3" s="7"/>
-      <c r="AS3" s="7"/>
-      <c r="AT3" s="0" t="n">
+      <c r="BC3" s="0" t="n">
         <v>719</v>
       </c>
-      <c r="AU3" s="7"/>
-      <c r="AV3" s="7"/>
-      <c r="AW3" s="7"/>
-      <c r="AX3" s="0" t="n">
+      <c r="BH3" s="0" t="n">
         <v>686.9</v>
       </c>
-      <c r="AY3" s="7"/>
-      <c r="AZ3" s="7"/>
-      <c r="BA3" s="7"/>
-      <c r="BB3" s="0" t="n">
+      <c r="BM3" s="0" t="n">
         <v>802.8</v>
       </c>
-      <c r="BC3" s="7"/>
-      <c r="BD3" s="7"/>
-      <c r="BE3" s="7"/>
-      <c r="BF3" s="0" t="n">
+      <c r="BR3" s="0" t="n">
         <v>931.4</v>
       </c>
-      <c r="BG3" s="7"/>
-      <c r="BH3" s="7"/>
-      <c r="BI3" s="7"/>
-      <c r="BJ3" s="0" t="n">
+      <c r="BW3" s="0" t="n">
         <v>1036.3</v>
       </c>
-      <c r="BK3" s="7"/>
-      <c r="BL3" s="7"/>
-      <c r="BM3" s="7"/>
-      <c r="BN3" s="0" t="n">
+      <c r="CB3" s="0" t="n">
         <v>1176</v>
       </c>
-      <c r="BO3" s="7"/>
-      <c r="BP3" s="7"/>
-      <c r="BQ3" s="7"/>
-      <c r="BR3" s="0" t="n">
+      <c r="CG3" s="0" t="n">
         <v>1232.9</v>
       </c>
-      <c r="BS3" s="7"/>
-      <c r="BT3" s="7"/>
-      <c r="BU3" s="7"/>
-      <c r="BV3" s="0" t="n">
+      <c r="CL3" s="0" t="n">
         <v>1339.4</v>
       </c>
-      <c r="BW3" s="7"/>
-      <c r="BX3" s="7"/>
-      <c r="BY3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1521</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E4" s="5" t="n">
         <v>44784</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
       <c r="J4" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="0" t="n">
+      <c r="O4" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="0" t="n">
+      <c r="T4" s="0" t="n">
         <v>132</v>
       </c>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="0" t="n">
+      <c r="Y4" s="0" t="n">
         <v>235.2</v>
       </c>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="0" t="n">
+      <c r="AD4" s="0" t="n">
         <v>331.4</v>
       </c>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="0" t="n">
+      <c r="AI4" s="0" t="n">
         <v>439</v>
       </c>
-      <c r="AE4" s="7"/>
-      <c r="AF4" s="7"/>
-      <c r="AG4" s="7"/>
-      <c r="AH4" s="0" t="n">
+      <c r="AN4" s="0" t="n">
         <v>551.6</v>
       </c>
-      <c r="AI4" s="7"/>
-      <c r="AJ4" s="7"/>
-      <c r="AK4" s="7"/>
-      <c r="AL4" s="0" t="n">
+      <c r="AS4" s="0" t="n">
         <v>627.3</v>
       </c>
-      <c r="AM4" s="7"/>
-      <c r="AN4" s="7"/>
-      <c r="AO4" s="7"/>
-      <c r="AP4" s="0" t="n">
+      <c r="AX4" s="0" t="n">
         <v>656.2</v>
       </c>
-      <c r="AQ4" s="7"/>
-      <c r="AR4" s="7"/>
-      <c r="AS4" s="7"/>
-      <c r="AT4" s="0" t="n">
+      <c r="BC4" s="0" t="n">
         <v>755.5</v>
       </c>
-      <c r="AU4" s="7"/>
-      <c r="AV4" s="7"/>
-      <c r="AW4" s="7"/>
-      <c r="AX4" s="0" t="n">
+      <c r="BH4" s="0" t="n">
         <v>847.1</v>
       </c>
-      <c r="AY4" s="7"/>
-      <c r="AZ4" s="7"/>
-      <c r="BA4" s="7"/>
-      <c r="BB4" s="0" t="n">
+      <c r="BM4" s="0" t="n">
         <v>985.4</v>
       </c>
-      <c r="BC4" s="7"/>
-      <c r="BD4" s="7"/>
-      <c r="BE4" s="7"/>
-      <c r="BF4" s="0" t="n">
+      <c r="BR4" s="0" t="n">
         <v>1062.6</v>
       </c>
-      <c r="BG4" s="7"/>
-      <c r="BH4" s="7"/>
-      <c r="BI4" s="7"/>
-      <c r="BJ4" s="0" t="n">
+      <c r="BW4" s="0" t="n">
         <v>1200.6</v>
       </c>
-      <c r="BK4" s="7"/>
-      <c r="BL4" s="7"/>
-      <c r="BM4" s="7"/>
-      <c r="BN4" s="0" t="n">
+      <c r="CB4" s="0" t="n">
         <v>1327</v>
       </c>
-      <c r="BO4" s="7"/>
-      <c r="BP4" s="7"/>
-      <c r="BQ4" s="7"/>
-      <c r="BR4" s="0" t="n">
+      <c r="CG4" s="0" t="n">
         <v>1363</v>
       </c>
-      <c r="BS4" s="7"/>
-      <c r="BT4" s="7"/>
-      <c r="BU4" s="7"/>
-      <c r="BV4" s="0" t="n">
+      <c r="CL4" s="0" t="n">
         <v>1452.4</v>
       </c>
-      <c r="BW4" s="7"/>
-      <c r="BX4" s="7"/>
-      <c r="BY4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>1522</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E5" s="5" t="n">
         <v>44784</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
       <c r="J5" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="0" t="n">
+      <c r="O5" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="0" t="n">
+      <c r="T5" s="0" t="n">
         <v>136</v>
       </c>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="0" t="n">
+      <c r="Y5" s="0" t="n">
         <v>246.6</v>
       </c>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="0" t="n">
+      <c r="AD5" s="0" t="n">
         <v>338.7</v>
       </c>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="0" t="n">
+      <c r="AI5" s="0" t="n">
         <v>457.5</v>
       </c>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="0" t="n">
+      <c r="AN5" s="0" t="n">
         <v>558.7</v>
       </c>
-      <c r="AI5" s="7"/>
-      <c r="AJ5" s="7"/>
-      <c r="AK5" s="7"/>
-      <c r="AL5" s="0" t="n">
+      <c r="AS5" s="0" t="n">
         <v>656</v>
       </c>
-      <c r="AM5" s="7"/>
-      <c r="AN5" s="7"/>
-      <c r="AO5" s="7"/>
-      <c r="AP5" s="0" t="n">
+      <c r="AX5" s="0" t="n">
         <v>616</v>
       </c>
-      <c r="AQ5" s="7"/>
-      <c r="AR5" s="7"/>
-      <c r="AS5" s="7"/>
-      <c r="AT5" s="0" t="n">
+      <c r="BC5" s="0" t="n">
         <v>712.9</v>
       </c>
-      <c r="AU5" s="7"/>
-      <c r="AV5" s="7"/>
-      <c r="AW5" s="7"/>
-      <c r="AX5" s="0" t="n">
+      <c r="BH5" s="0" t="n">
         <v>756.1</v>
       </c>
-      <c r="AY5" s="7"/>
-      <c r="AZ5" s="7"/>
-      <c r="BA5" s="7"/>
-      <c r="BB5" s="0" t="n">
+      <c r="BM5" s="0" t="n">
         <v>856.5</v>
       </c>
-      <c r="BC5" s="7"/>
-      <c r="BD5" s="7"/>
-      <c r="BE5" s="7"/>
-      <c r="BF5" s="0" t="n">
+      <c r="BR5" s="0" t="n">
         <v>1061</v>
       </c>
-      <c r="BG5" s="7"/>
-      <c r="BH5" s="7"/>
-      <c r="BI5" s="7"/>
-      <c r="BJ5" s="0" t="n">
+      <c r="BW5" s="0" t="n">
         <v>1195</v>
       </c>
-      <c r="BK5" s="7"/>
-      <c r="BL5" s="7"/>
-      <c r="BM5" s="7"/>
-      <c r="BN5" s="0" t="n">
+      <c r="CB5" s="0" t="n">
         <v>1358.1</v>
       </c>
-      <c r="BO5" s="7"/>
-      <c r="BP5" s="7"/>
-      <c r="BQ5" s="7"/>
-      <c r="BR5" s="0" t="n">
+      <c r="CG5" s="0" t="n">
         <v>1412.5</v>
       </c>
-      <c r="BS5" s="7"/>
-      <c r="BT5" s="7"/>
-      <c r="BU5" s="7"/>
-      <c r="BV5" s="0" t="n">
+      <c r="CL5" s="0" t="n">
         <v>1450</v>
       </c>
-      <c r="BW5" s="7"/>
-      <c r="BX5" s="7"/>
-      <c r="BY5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>1523</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="n">
         <v>44784</v>
       </c>
+      <c r="F6" s="1"/>
       <c r="J6" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="O6" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="R6" s="0" t="n">
+      <c r="T6" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="V6" s="0" t="n">
+      <c r="Y6" s="0" t="n">
         <v>207.8</v>
       </c>
-      <c r="Z6" s="0" t="n">
+      <c r="AD6" s="0" t="n">
         <v>287.9</v>
       </c>
-      <c r="AD6" s="0" t="n">
+      <c r="AI6" s="0" t="n">
         <v>409.7</v>
       </c>
-      <c r="AH6" s="0" t="n">
+      <c r="AN6" s="0" t="n">
         <v>520.6</v>
       </c>
-      <c r="AL6" s="0" t="n">
+      <c r="AS6" s="0" t="n">
         <v>610</v>
       </c>
-      <c r="AP6" s="0" t="n">
+      <c r="AX6" s="0" t="n">
         <v>654.1</v>
       </c>
-      <c r="AT6" s="0" t="n">
+      <c r="BC6" s="0" t="n">
         <v>737.7</v>
       </c>
-      <c r="AX6" s="0" t="n">
+      <c r="BH6" s="0" t="n">
         <v>959.3</v>
       </c>
-      <c r="BB6" s="0" t="n">
+      <c r="BM6" s="0" t="n">
         <v>1133.9</v>
       </c>
-      <c r="BF6" s="0" t="n">
+      <c r="BR6" s="0" t="n">
         <v>1211.7</v>
       </c>
-      <c r="BJ6" s="0" t="n">
+      <c r="BW6" s="0" t="n">
         <v>1378.8</v>
       </c>
-      <c r="BN6" s="0" t="n">
+      <c r="CB6" s="0" t="n">
         <v>1513.5</v>
       </c>
-      <c r="BR6" s="8" t="n">
+      <c r="CG6" s="6" t="n">
         <v>1618.1</v>
       </c>
-      <c r="BV6" s="0" t="n">
+      <c r="CL6" s="0" t="n">
         <v>1792.2</v>
       </c>
     </row>
@@ -1167,60 +1061,60 @@
         <v>1524</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="E7" s="5" t="n">
         <v>44784</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="O7" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="R7" s="0" t="n">
+      <c r="T7" s="0" t="n">
         <v>155</v>
       </c>
-      <c r="V7" s="0" t="n">
+      <c r="Y7" s="0" t="n">
         <v>286.1</v>
       </c>
-      <c r="Z7" s="0" t="n">
+      <c r="AD7" s="0" t="n">
         <v>410.2</v>
       </c>
-      <c r="AD7" s="0" t="n">
+      <c r="AI7" s="0" t="n">
         <v>551.2</v>
       </c>
-      <c r="AH7" s="0" t="n">
+      <c r="AN7" s="0" t="n">
         <v>688.3</v>
       </c>
-      <c r="AL7" s="0" t="n">
+      <c r="AS7" s="0" t="n">
         <v>768</v>
       </c>
-      <c r="AP7" s="0" t="n">
+      <c r="AX7" s="0" t="n">
         <v>776.4</v>
       </c>
-      <c r="AT7" s="0" t="n">
+      <c r="BC7" s="0" t="n">
         <v>889.2</v>
       </c>
-      <c r="AX7" s="0" t="n">
+      <c r="BH7" s="0" t="n">
         <v>1140</v>
       </c>
-      <c r="BB7" s="0" t="n">
+      <c r="BM7" s="0" t="n">
         <v>1321.4</v>
       </c>
-      <c r="BF7" s="0" t="n">
+      <c r="BR7" s="0" t="n">
         <v>1435.3</v>
       </c>
-      <c r="BJ7" s="0" t="n">
+      <c r="BW7" s="0" t="n">
         <v>1592.3</v>
       </c>
-      <c r="BN7" s="0" t="n">
+      <c r="CB7" s="0" t="n">
         <v>1806</v>
       </c>
-      <c r="BR7" s="0" t="n">
+      <c r="CG7" s="0" t="n">
         <v>1844.8</v>
       </c>
-      <c r="BV7" s="0" t="n">
+      <c r="CL7" s="0" t="n">
         <v>1984.8</v>
       </c>
     </row>
@@ -1229,60 +1123,61 @@
         <v>1525</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="E8" s="5" t="n">
         <v>44784</v>
       </c>
-      <c r="J8" s="9" t="n">
+      <c r="F8" s="1"/>
+      <c r="J8" s="7" t="n">
         <v>43</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="O8" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="R8" s="0" t="n">
+      <c r="T8" s="0" t="n">
         <v>167</v>
       </c>
-      <c r="V8" s="0" t="n">
+      <c r="Y8" s="0" t="n">
         <v>297.7</v>
       </c>
-      <c r="Z8" s="0" t="n">
+      <c r="AD8" s="0" t="n">
         <v>446.2</v>
       </c>
-      <c r="AD8" s="0" t="n">
+      <c r="AI8" s="0" t="n">
         <v>605.5</v>
       </c>
-      <c r="AH8" s="0" t="n">
+      <c r="AN8" s="0" t="n">
         <v>735.3</v>
       </c>
-      <c r="AL8" s="0" t="n">
+      <c r="AS8" s="0" t="n">
         <v>890</v>
       </c>
-      <c r="AP8" s="0" t="n">
+      <c r="AX8" s="0" t="n">
         <v>914.6</v>
       </c>
-      <c r="AT8" s="0" t="n">
+      <c r="BC8" s="0" t="n">
         <v>1064.6</v>
       </c>
-      <c r="AX8" s="0" t="n">
+      <c r="BH8" s="0" t="n">
         <v>1065.3</v>
       </c>
-      <c r="BB8" s="0" t="n">
+      <c r="BM8" s="0" t="n">
         <v>1254.1</v>
       </c>
-      <c r="BF8" s="0" t="n">
+      <c r="BR8" s="0" t="n">
         <v>1420</v>
       </c>
-      <c r="BJ8" s="0" t="n">
+      <c r="BW8" s="0" t="n">
         <v>1669.6</v>
       </c>
-      <c r="BN8" s="0" t="n">
+      <c r="CB8" s="0" t="n">
         <v>1800</v>
       </c>
-      <c r="BR8" s="0" t="n">
+      <c r="CG8" s="0" t="n">
         <v>1907.6</v>
       </c>
-      <c r="BV8" s="0" t="n">
+      <c r="CL8" s="0" t="n">
         <v>2090.8</v>
       </c>
     </row>
@@ -1291,71 +1186,72 @@
         <v>1526</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E9" s="5" t="n">
         <v>44784</v>
       </c>
+      <c r="F9" s="1"/>
       <c r="J9" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="O9" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="R9" s="0" t="n">
+      <c r="T9" s="0" t="n">
         <v>172</v>
       </c>
-      <c r="V9" s="0" t="n">
+      <c r="Y9" s="0" t="n">
         <v>297.2</v>
       </c>
-      <c r="Z9" s="0" t="n">
+      <c r="AD9" s="0" t="n">
         <v>395.4</v>
       </c>
-      <c r="AD9" s="0" t="n">
+      <c r="AI9" s="0" t="n">
         <v>521</v>
       </c>
-      <c r="AH9" s="0" t="n">
+      <c r="AN9" s="0" t="n">
         <v>628.1</v>
       </c>
-      <c r="AL9" s="0" t="n">
+      <c r="AS9" s="0" t="n">
         <v>717.4</v>
       </c>
-      <c r="AP9" s="0" t="n">
+      <c r="AX9" s="0" t="n">
         <v>619.7</v>
       </c>
-      <c r="AT9" s="0" t="n">
+      <c r="BC9" s="0" t="n">
         <v>783.2</v>
       </c>
-      <c r="AX9" s="0" t="n">
+      <c r="BH9" s="0" t="n">
         <v>875.6</v>
       </c>
-      <c r="BB9" s="0" t="n">
+      <c r="BM9" s="0" t="n">
         <v>1036.4</v>
       </c>
-      <c r="BF9" s="0" t="n">
+      <c r="BR9" s="0" t="n">
         <v>1175.2</v>
       </c>
-      <c r="BJ9" s="0" t="n">
+      <c r="BW9" s="0" t="n">
         <v>1351.6</v>
       </c>
-      <c r="BN9" s="0" t="n">
+      <c r="CB9" s="0" t="n">
         <v>1444.4</v>
       </c>
-      <c r="BR9" s="0" t="n">
+      <c r="CG9" s="0" t="n">
         <v>1480.6</v>
       </c>
-      <c r="BV9" s="0" t="n">
+      <c r="CL9" s="0" t="n">
         <v>1529.9</v>
       </c>
     </row>
-    <row r="10" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>1527</v>
       </c>
       <c r="B10" s="0"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="6" t="n">
+      <c r="E10" s="5" t="n">
         <v>44784</v>
       </c>
       <c r="F10" s="1"/>
@@ -1368,81 +1264,81 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="0" t="n">
+      <c r="N10" s="1"/>
+      <c r="O10" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="0" t="n">
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="0" t="n">
         <v>142</v>
       </c>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
       <c r="U10" s="1"/>
-      <c r="V10" s="0" t="n">
-        <v>231.8</v>
-      </c>
+      <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="0" t="n">
-        <v>350.2</v>
-      </c>
+      <c r="Y10" s="0" t="n">
+        <v>231.8</v>
+      </c>
+      <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="0" t="n">
-        <v>465.5</v>
+        <v>350.2</v>
       </c>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
-      <c r="AH10" s="0" t="n">
-        <v>557.6</v>
-      </c>
-      <c r="AI10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="0" t="n">
+        <v>465.5</v>
+      </c>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
-      <c r="AL10" s="0" t="n">
-        <v>691.5</v>
-      </c>
+      <c r="AL10" s="1"/>
       <c r="AM10" s="1"/>
-      <c r="AN10" s="1"/>
+      <c r="AN10" s="0" t="n">
+        <v>557.6</v>
+      </c>
       <c r="AO10" s="1"/>
-      <c r="AP10" s="0" t="n">
-        <v>728.9</v>
-      </c>
+      <c r="AP10" s="1"/>
       <c r="AQ10" s="1"/>
       <c r="AR10" s="1"/>
-      <c r="AS10" s="1"/>
-      <c r="AT10" s="0" t="n">
-        <v>869</v>
-      </c>
+      <c r="AS10" s="0" t="n">
+        <v>691.5</v>
+      </c>
+      <c r="AT10" s="1"/>
       <c r="AU10" s="1"/>
       <c r="AV10" s="1"/>
       <c r="AW10" s="1"/>
       <c r="AX10" s="0" t="n">
-        <v>1013.1</v>
+        <v>728.9</v>
       </c>
       <c r="AY10" s="1"/>
       <c r="AZ10" s="1"/>
       <c r="BA10" s="1"/>
-      <c r="BB10" s="0" t="n">
-        <v>1197</v>
-      </c>
-      <c r="BC10" s="1"/>
+      <c r="BB10" s="1"/>
+      <c r="BC10" s="0" t="n">
+        <v>869</v>
+      </c>
       <c r="BD10" s="1"/>
       <c r="BE10" s="1"/>
-      <c r="BF10" s="0"/>
+      <c r="BF10" s="1"/>
       <c r="BG10" s="1"/>
-      <c r="BH10" s="1"/>
+      <c r="BH10" s="0" t="n">
+        <v>1013.1</v>
+      </c>
       <c r="BI10" s="1"/>
-      <c r="BJ10" s="0"/>
+      <c r="BJ10" s="1"/>
       <c r="BK10" s="1"/>
       <c r="BL10" s="1"/>
-      <c r="BM10" s="1"/>
-      <c r="BN10" s="0"/>
+      <c r="BM10" s="0" t="n">
+        <v>1197</v>
+      </c>
+      <c r="BN10" s="1"/>
       <c r="BO10" s="1"/>
       <c r="BP10" s="1"/>
       <c r="BQ10" s="1"/>
@@ -1450,70 +1346,92 @@
       <c r="BS10" s="1"/>
       <c r="BT10" s="1"/>
       <c r="BU10" s="1"/>
-      <c r="BV10" s="0"/>
-      <c r="BW10" s="1"/>
+      <c r="BV10" s="1"/>
+      <c r="BW10" s="0"/>
       <c r="BX10" s="1"/>
       <c r="BY10" s="1"/>
+      <c r="BZ10" s="1"/>
+      <c r="CA10" s="1"/>
+      <c r="CB10" s="0"/>
+      <c r="CC10" s="1"/>
+      <c r="CD10" s="1"/>
+      <c r="CE10" s="1"/>
+      <c r="CF10" s="1"/>
+      <c r="CG10" s="0"/>
+      <c r="CH10" s="1"/>
+      <c r="CI10" s="1"/>
+      <c r="CJ10" s="1"/>
+      <c r="CK10" s="1"/>
+      <c r="CL10" s="0"/>
+      <c r="CM10" s="1"/>
+      <c r="CN10" s="1"/>
+      <c r="CO10" s="1"/>
+      <c r="CP10" s="1"/>
+      <c r="CQ10" s="0"/>
+      <c r="CR10" s="0"/>
+      <c r="CS10" s="0"/>
+      <c r="CT10" s="0"/>
+      <c r="CU10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>1528</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="E11" s="5" t="n">
         <v>44784</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="O11" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="R11" s="0" t="n">
+      <c r="T11" s="0" t="n">
         <v>175</v>
       </c>
-      <c r="V11" s="0" t="n">
+      <c r="Y11" s="0" t="n">
         <v>309.5</v>
       </c>
-      <c r="Z11" s="0" t="n">
+      <c r="AD11" s="0" t="n">
         <v>451.4</v>
       </c>
-      <c r="AD11" s="0" t="n">
+      <c r="AI11" s="0" t="n">
         <v>617.8</v>
       </c>
-      <c r="AH11" s="0" t="n">
+      <c r="AN11" s="0" t="n">
         <v>743.1</v>
       </c>
-      <c r="AL11" s="0" t="n">
+      <c r="AS11" s="0" t="n">
         <v>921</v>
       </c>
-      <c r="AP11" s="0" t="n">
+      <c r="AX11" s="0" t="n">
         <v>979.1</v>
       </c>
-      <c r="AT11" s="0" t="n">
+      <c r="BC11" s="0" t="n">
         <v>1124.7</v>
       </c>
-      <c r="AX11" s="0" t="n">
+      <c r="BH11" s="0" t="n">
         <v>1149.2</v>
       </c>
-      <c r="BB11" s="0" t="n">
+      <c r="BM11" s="0" t="n">
         <v>1617.1</v>
       </c>
-      <c r="BF11" s="0" t="n">
+      <c r="BR11" s="0" t="n">
         <v>1832.6</v>
       </c>
-      <c r="BJ11" s="0" t="n">
+      <c r="BW11" s="0" t="n">
         <v>1935.9</v>
       </c>
-      <c r="BN11" s="0" t="n">
+      <c r="CB11" s="0" t="n">
         <v>2133.7</v>
       </c>
-      <c r="BR11" s="0" t="n">
+      <c r="CG11" s="0" t="n">
         <v>2212.8</v>
       </c>
-      <c r="BV11" s="0" t="n">
+      <c r="CL11" s="0" t="n">
         <v>2308.2</v>
       </c>
     </row>
@@ -1522,60 +1440,60 @@
         <v>1529</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E12" s="5" t="n">
         <v>44784</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="O12" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="R12" s="0" t="n">
+      <c r="T12" s="0" t="n">
         <v>86</v>
       </c>
-      <c r="V12" s="0" t="n">
+      <c r="Y12" s="0" t="n">
         <v>157.7</v>
       </c>
-      <c r="Z12" s="0" t="n">
+      <c r="AD12" s="0" t="n">
         <v>236.4</v>
       </c>
-      <c r="AD12" s="0" t="n">
+      <c r="AI12" s="0" t="n">
         <v>318.7</v>
       </c>
-      <c r="AH12" s="0" t="n">
+      <c r="AN12" s="0" t="n">
         <v>406.9</v>
       </c>
-      <c r="AL12" s="0" t="n">
+      <c r="AS12" s="0" t="n">
         <v>485.9</v>
       </c>
-      <c r="AP12" s="0" t="n">
+      <c r="AX12" s="0" t="n">
         <v>484.4</v>
       </c>
-      <c r="AT12" s="0" t="n">
+      <c r="BC12" s="0" t="n">
         <v>567.9</v>
       </c>
-      <c r="AX12" s="0" t="n">
+      <c r="BH12" s="0" t="n">
         <v>712.3</v>
       </c>
-      <c r="BB12" s="0" t="n">
+      <c r="BM12" s="0" t="n">
         <v>843.3</v>
       </c>
-      <c r="BF12" s="0" t="n">
+      <c r="BR12" s="0" t="n">
         <v>838.6</v>
       </c>
-      <c r="BJ12" s="0" t="n">
+      <c r="BW12" s="0" t="n">
         <v>969.3</v>
       </c>
-      <c r="BN12" s="0" t="n">
+      <c r="CB12" s="0" t="n">
         <v>1085.1</v>
       </c>
-      <c r="BR12" s="0" t="n">
+      <c r="CG12" s="0" t="n">
         <v>1141.5</v>
       </c>
-      <c r="BV12" s="0" t="n">
+      <c r="CL12" s="0" t="n">
         <v>1243.8</v>
       </c>
     </row>
@@ -1584,60 +1502,60 @@
         <v>1530</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="E13" s="5" t="n">
         <v>44784</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="O13" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="R13" s="0" t="n">
+      <c r="T13" s="0" t="n">
         <v>162</v>
       </c>
-      <c r="V13" s="0" t="n">
+      <c r="Y13" s="0" t="n">
         <v>287.1</v>
       </c>
-      <c r="Z13" s="0" t="n">
+      <c r="AD13" s="0" t="n">
         <v>415.3</v>
       </c>
-      <c r="AD13" s="0" t="n">
+      <c r="AI13" s="0" t="n">
         <v>578.5</v>
       </c>
-      <c r="AH13" s="0" t="n">
+      <c r="AN13" s="0" t="n">
         <v>727.9</v>
       </c>
-      <c r="AL13" s="0" t="n">
+      <c r="AS13" s="0" t="n">
         <v>880</v>
       </c>
-      <c r="AP13" s="0" t="n">
+      <c r="AX13" s="0" t="n">
         <v>894.5</v>
       </c>
-      <c r="AT13" s="0" t="n">
+      <c r="BC13" s="0" t="n">
         <v>1053.7</v>
       </c>
-      <c r="AX13" s="0" t="n">
+      <c r="BH13" s="0" t="n">
         <v>1189.1</v>
       </c>
-      <c r="BB13" s="0" t="n">
+      <c r="BM13" s="0" t="n">
         <v>1414.9</v>
       </c>
-      <c r="BF13" s="0" t="n">
+      <c r="BR13" s="0" t="n">
         <v>1547.4</v>
       </c>
-      <c r="BJ13" s="0" t="n">
+      <c r="BW13" s="0" t="n">
         <v>1808.6</v>
       </c>
-      <c r="BN13" s="0" t="n">
+      <c r="CB13" s="0" t="n">
         <v>1781</v>
       </c>
-      <c r="BR13" s="0" t="n">
+      <c r="CG13" s="0" t="n">
         <v>1852</v>
       </c>
-      <c r="BV13" s="0" t="n">
+      <c r="CL13" s="0" t="n">
         <v>1879.4</v>
       </c>
     </row>
@@ -1646,60 +1564,60 @@
         <v>1531</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="E14" s="5" t="n">
         <v>44784</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="N14" s="0" t="n">
+      <c r="O14" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="R14" s="0" t="n">
+      <c r="T14" s="0" t="n">
         <v>118</v>
       </c>
-      <c r="V14" s="0" t="n">
+      <c r="Y14" s="0" t="n">
         <v>218.7</v>
       </c>
-      <c r="Z14" s="0" t="n">
+      <c r="AD14" s="0" t="n">
         <v>318.3</v>
       </c>
-      <c r="AD14" s="0" t="n">
+      <c r="AI14" s="0" t="n">
         <v>447.8</v>
       </c>
-      <c r="AH14" s="0" t="n">
+      <c r="AN14" s="0" t="n">
         <v>545.5</v>
       </c>
-      <c r="AL14" s="0" t="n">
+      <c r="AS14" s="0" t="n">
         <v>655</v>
       </c>
-      <c r="AP14" s="0" t="n">
+      <c r="AX14" s="0" t="n">
         <v>721.4</v>
       </c>
-      <c r="AT14" s="0" t="n">
+      <c r="BC14" s="0" t="n">
         <v>836</v>
       </c>
-      <c r="AX14" s="0" t="n">
+      <c r="BH14" s="0" t="n">
         <v>1031.2</v>
       </c>
-      <c r="BB14" s="0" t="n">
+      <c r="BM14" s="0" t="n">
         <v>1223.2</v>
       </c>
-      <c r="BF14" s="0" t="n">
+      <c r="BR14" s="0" t="n">
         <v>1342</v>
       </c>
-      <c r="BJ14" s="0" t="n">
+      <c r="BW14" s="0" t="n">
         <v>1562.9</v>
       </c>
-      <c r="BN14" s="0" t="n">
+      <c r="CB14" s="0" t="n">
         <v>1685.8</v>
       </c>
-      <c r="BR14" s="0" t="n">
+      <c r="CG14" s="0" t="n">
         <v>1730.5</v>
       </c>
-      <c r="BV14" s="0" t="n">
+      <c r="CL14" s="0" t="n">
         <v>1853.7</v>
       </c>
     </row>
@@ -1708,60 +1626,60 @@
         <v>1532</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="E15" s="5" t="n">
         <v>44784</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="O15" s="0" t="n">
         <v>77</v>
       </c>
-      <c r="R15" s="0" t="n">
+      <c r="T15" s="0" t="n">
         <v>134</v>
       </c>
-      <c r="V15" s="0" t="n">
+      <c r="Y15" s="0" t="n">
         <v>241.5</v>
       </c>
-      <c r="Z15" s="0" t="n">
+      <c r="AD15" s="0" t="n">
         <v>356.7</v>
       </c>
-      <c r="AD15" s="0" t="n">
+      <c r="AI15" s="0" t="n">
         <v>506.8</v>
       </c>
-      <c r="AH15" s="0" t="n">
+      <c r="AN15" s="0" t="n">
         <v>631.3</v>
       </c>
-      <c r="AL15" s="0" t="n">
+      <c r="AS15" s="0" t="n">
         <v>741.3</v>
       </c>
-      <c r="AP15" s="8" t="n">
+      <c r="AX15" s="6" t="n">
         <v>757.8</v>
       </c>
-      <c r="AT15" s="0" t="n">
+      <c r="BC15" s="0" t="n">
         <v>905</v>
       </c>
-      <c r="AX15" s="0" t="n">
+      <c r="BH15" s="0" t="n">
         <v>1140</v>
       </c>
-      <c r="BB15" s="0" t="n">
+      <c r="BM15" s="0" t="n">
         <v>1320.2</v>
       </c>
-      <c r="BF15" s="0" t="n">
+      <c r="BR15" s="0" t="n">
         <v>1466.2</v>
       </c>
-      <c r="BJ15" s="0" t="n">
+      <c r="BW15" s="0" t="n">
         <v>1691.3</v>
       </c>
-      <c r="BN15" s="0" t="n">
+      <c r="CB15" s="0" t="n">
         <v>1971</v>
       </c>
-      <c r="BR15" s="0" t="n">
+      <c r="CG15" s="0" t="n">
         <v>2039.1</v>
       </c>
-      <c r="BV15" s="0" t="n">
+      <c r="CL15" s="0" t="n">
         <v>2214.9</v>
       </c>
     </row>
@@ -1770,60 +1688,60 @@
         <v>1533</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E16" s="5" t="n">
         <v>44784</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="N16" s="0" t="n">
+      <c r="O16" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="R16" s="0" t="n">
+      <c r="T16" s="0" t="n">
         <v>142</v>
       </c>
-      <c r="V16" s="0" t="n">
+      <c r="Y16" s="0" t="n">
         <v>228.7</v>
       </c>
-      <c r="Z16" s="0" t="n">
+      <c r="AD16" s="0" t="n">
         <v>328.4</v>
       </c>
-      <c r="AD16" s="0" t="n">
+      <c r="AI16" s="0" t="n">
         <v>454.3</v>
       </c>
-      <c r="AH16" s="0" t="n">
+      <c r="AN16" s="0" t="n">
         <v>561.5</v>
       </c>
-      <c r="AL16" s="0" t="n">
+      <c r="AS16" s="0" t="n">
         <v>687.5</v>
       </c>
-      <c r="AP16" s="0" t="n">
+      <c r="AX16" s="0" t="n">
         <v>593.4</v>
       </c>
-      <c r="AT16" s="0" t="n">
+      <c r="BC16" s="0" t="n">
         <v>717.8</v>
       </c>
-      <c r="AX16" s="0" t="n">
+      <c r="BH16" s="0" t="n">
         <v>899</v>
       </c>
-      <c r="BB16" s="0" t="n">
+      <c r="BM16" s="0" t="n">
         <v>1072.2</v>
       </c>
-      <c r="BF16" s="0" t="n">
+      <c r="BR16" s="0" t="n">
         <v>1252</v>
       </c>
-      <c r="BJ16" s="0" t="n">
+      <c r="BW16" s="0" t="n">
         <v>1592.6</v>
       </c>
-      <c r="BN16" s="0" t="n">
+      <c r="CB16" s="0" t="n">
         <v>1495.1</v>
       </c>
-      <c r="BR16" s="0" t="n">
+      <c r="CG16" s="0" t="n">
         <v>1554.6</v>
       </c>
-      <c r="BV16" s="0" t="n">
+      <c r="CL16" s="0" t="n">
         <v>1655.3</v>
       </c>
     </row>
@@ -1832,60 +1750,60 @@
         <v>1534</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E17" s="5" t="n">
         <v>44784</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="N17" s="0" t="n">
+      <c r="O17" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="R17" s="0" t="n">
+      <c r="T17" s="0" t="n">
         <v>128</v>
       </c>
-      <c r="V17" s="0" t="n">
+      <c r="Y17" s="0" t="n">
         <v>199.5</v>
       </c>
-      <c r="Z17" s="0" t="n">
+      <c r="AD17" s="0" t="n">
         <v>289.4</v>
       </c>
-      <c r="AD17" s="0" t="n">
+      <c r="AI17" s="0" t="n">
         <v>395.4</v>
       </c>
-      <c r="AH17" s="0" t="n">
+      <c r="AN17" s="0" t="n">
         <v>507.8</v>
       </c>
-      <c r="AL17" s="0" t="n">
+      <c r="AS17" s="0" t="n">
         <v>625.6</v>
       </c>
-      <c r="AP17" s="0" t="n">
+      <c r="AX17" s="0" t="n">
         <v>608.6</v>
       </c>
-      <c r="AT17" s="0" t="n">
+      <c r="BC17" s="0" t="n">
         <v>740.1</v>
       </c>
-      <c r="AX17" s="0" t="n">
+      <c r="BH17" s="0" t="n">
         <v>894.2</v>
       </c>
-      <c r="BB17" s="0" t="n">
+      <c r="BM17" s="0" t="n">
         <v>1050.9</v>
       </c>
-      <c r="BF17" s="0" t="n">
+      <c r="BR17" s="0" t="n">
         <v>1184.4</v>
       </c>
-      <c r="BJ17" s="0" t="n">
+      <c r="BW17" s="0" t="n">
         <v>1334</v>
       </c>
-      <c r="BN17" s="0" t="n">
+      <c r="CB17" s="0" t="n">
         <v>1417.3</v>
       </c>
-      <c r="BR17" s="0" t="n">
+      <c r="CG17" s="0" t="n">
         <v>1525.1</v>
       </c>
-      <c r="BV17" s="0" t="n">
+      <c r="CL17" s="0" t="n">
         <v>1665.1</v>
       </c>
     </row>
@@ -1894,60 +1812,60 @@
         <v>1535</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="E18" s="5" t="n">
         <v>44784</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="N18" s="0" t="n">
+      <c r="O18" s="0" t="n">
         <v>77</v>
       </c>
-      <c r="R18" s="0" t="n">
+      <c r="T18" s="0" t="n">
         <v>142</v>
       </c>
-      <c r="V18" s="0" t="n">
+      <c r="Y18" s="0" t="n">
         <v>248.2</v>
       </c>
-      <c r="Z18" s="0" t="n">
+      <c r="AD18" s="0" t="n">
         <v>353.6</v>
       </c>
-      <c r="AD18" s="0" t="n">
+      <c r="AI18" s="0" t="n">
         <v>482.1</v>
       </c>
-      <c r="AH18" s="0" t="n">
+      <c r="AN18" s="0" t="n">
         <v>621.2</v>
       </c>
-      <c r="AL18" s="0" t="n">
+      <c r="AS18" s="0" t="n">
         <v>740.7</v>
       </c>
-      <c r="AP18" s="0" t="n">
+      <c r="AX18" s="0" t="n">
         <v>656.1</v>
       </c>
-      <c r="AT18" s="0" t="n">
+      <c r="BC18" s="0" t="n">
         <v>786.7</v>
       </c>
-      <c r="AX18" s="0" t="n">
+      <c r="BH18" s="0" t="n">
         <v>938.1</v>
       </c>
-      <c r="BB18" s="0" t="n">
+      <c r="BM18" s="0" t="n">
         <v>979.6</v>
       </c>
-      <c r="BF18" s="0" t="n">
+      <c r="BR18" s="0" t="n">
         <v>1057.8</v>
       </c>
-      <c r="BJ18" s="0" t="n">
+      <c r="BW18" s="0" t="n">
         <v>1205.9</v>
       </c>
-      <c r="BN18" s="0" t="n">
+      <c r="CB18" s="0" t="n">
         <v>1285.7</v>
       </c>
-      <c r="BR18" s="0" t="n">
+      <c r="CG18" s="0" t="n">
         <v>1366.5</v>
       </c>
-      <c r="BV18" s="0" t="n">
+      <c r="CL18" s="0" t="n">
         <v>1510.3</v>
       </c>
     </row>
@@ -1956,83 +1874,83 @@
         <v>1536</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="E19" s="5" t="n">
         <v>44784</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="N19" s="0" t="n">
+      <c r="O19" s="0" t="n">
         <v>77</v>
       </c>
-      <c r="R19" s="0" t="n">
+      <c r="T19" s="0" t="n">
         <v>142</v>
       </c>
-      <c r="V19" s="0" t="n">
+      <c r="Y19" s="0" t="n">
         <v>273.3</v>
       </c>
-      <c r="Z19" s="0" t="n">
+      <c r="AD19" s="0" t="n">
         <v>396.7</v>
       </c>
-      <c r="AD19" s="0" t="n">
+      <c r="AI19" s="0" t="n">
         <v>537.6</v>
       </c>
-      <c r="AH19" s="0" t="n">
+      <c r="AN19" s="0" t="n">
         <v>667</v>
       </c>
-      <c r="AL19" s="0" t="n">
+      <c r="AS19" s="0" t="n">
         <v>819.9</v>
       </c>
-      <c r="AP19" s="0" t="n">
+      <c r="AX19" s="0" t="n">
         <v>751.2</v>
       </c>
-      <c r="AT19" s="0" t="n">
+      <c r="BC19" s="0" t="n">
         <v>873.6</v>
       </c>
-      <c r="AX19" s="0" t="n">
+      <c r="BH19" s="0" t="n">
         <v>1176.1</v>
       </c>
-      <c r="BB19" s="0" t="n">
+      <c r="BM19" s="0" t="n">
         <v>1405.8</v>
       </c>
-      <c r="BF19" s="0" t="n">
+      <c r="BR19" s="0" t="n">
         <v>1626.1</v>
       </c>
-      <c r="BJ19" s="0" t="n">
+      <c r="BW19" s="0" t="n">
         <v>1812.9</v>
       </c>
-      <c r="BN19" s="0" t="n">
+      <c r="CB19" s="0" t="n">
         <v>2057.8</v>
       </c>
-      <c r="BR19" s="0" t="n">
+      <c r="CG19" s="0" t="n">
         <v>2182.4</v>
       </c>
-      <c r="BV19" s="0" t="n">
+      <c r="CL19" s="0" t="n">
         <v>2341.8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="BV1:BY1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="O1:S1"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="Y1:AC1"/>
+    <mergeCell ref="AD1:AH1"/>
+    <mergeCell ref="AI1:AM1"/>
+    <mergeCell ref="AN1:AR1"/>
+    <mergeCell ref="AS1:AW1"/>
+    <mergeCell ref="AX1:BB1"/>
+    <mergeCell ref="BC1:BG1"/>
+    <mergeCell ref="BH1:BL1"/>
+    <mergeCell ref="BM1:BQ1"/>
+    <mergeCell ref="BR1:BV1"/>
+    <mergeCell ref="BW1:CA1"/>
+    <mergeCell ref="CB1:CF1"/>
+    <mergeCell ref="CG1:CK1"/>
+    <mergeCell ref="CL1:CP1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>